<commit_message>
Demand builder working in script now.  Had to fix typo and determine newlines based on host OS.
</commit_message>
<xml_diff>
--- a/resources/timeline_Colorado.xlsx
+++ b/resources/timeline_Colorado.xlsx
@@ -31,13 +31,13 @@
     <t xml:space="preserve">Duration</t>
   </si>
   <si>
-    <t xml:space="preserve">S-7337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S-706</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE-99</t>
+    <t xml:space="preserve">AlaskaFwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlaskaRot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE-Colorado</t>
   </si>
 </sst>
 </file>
@@ -52,6 +52,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,14 +137,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>